<commit_message>
Role in JwtDTO and visibility only for teachers
</commit_message>
<xml_diff>
--- a/manual_tests/browse_proposals_frontend.xlsx
+++ b/manual_tests/browse_proposals_frontend.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\manua\Desktop\SE2\thesis-management\manual_tests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DAC88C8-CFDE-4BAA-AFEB-572C67C342B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7957E144-D88D-4355-B78D-4B17A75E5E00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Feature</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Stop seeing details about the proposal</t>
+  </si>
+  <si>
+    <t>Do not see list of proposals if not logged in as teacher</t>
+  </si>
+  <si>
+    <t>Do not log in, go to home page</t>
+  </si>
+  <si>
+    <t>Sidebar should not contain link to browse proposals</t>
   </si>
 </sst>
 </file>
@@ -419,16 +428,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="A4:E4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.77734375" customWidth="1"/>
-    <col min="2" max="2" width="31.88671875" customWidth="1"/>
+    <col min="2" max="2" width="45.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.6640625" customWidth="1"/>
     <col min="4" max="4" width="26.77734375" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" customWidth="1"/>
@@ -502,6 +511,23 @@
         <v>45243</v>
       </c>
     </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="3">
+        <v>45243</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>